<commit_message>
Foi inserido os reports, os 3 cenarios de falha, o contexto nas feature e modo de tirar as screenshot.
</commit_message>
<xml_diff>
--- a/target/Excel/Dados.xlsx
+++ b/target/Excel/Dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus.vieira\ProjetoAvaliação\AdvantageShopBDD\target\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD036CB-883A-4A44-9DEB-54B4F2C9A63C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E1CD045-6585-444A-8198-076E7EB1C0D1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3510" yWindow="2295" windowWidth="15375" windowHeight="7875" xr2:uid="{E0E69BFF-8C0C-4BBC-880E-E66347D52EC9}"/>
   </bookViews>
@@ -143,7 +143,7 @@
     <t>HP Pro</t>
   </si>
   <si>
-    <t>Vergts</t>
+    <t>Printscreen5</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
alterado o metodo de selecionar o pais na criacao de conta, e alterado na feature, não passsa mas nenhuma String.
</commit_message>
<xml_diff>
--- a/target/Excel/Dados.xlsx
+++ b/target/Excel/Dados.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus.vieira\ProjetoAvaliação\AdvantageShopBDD\target\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus.vieira\ProjetoAdvantageBDD\AdvantageShopBDD\target\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E1CD045-6585-444A-8198-076E7EB1C0D1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F7CC65-620D-4817-BB7E-C492EF1E803C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="2295" windowWidth="15375" windowHeight="7875" xr2:uid="{E0E69BFF-8C0C-4BBC-880E-E66347D52EC9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E0E69BFF-8C0C-4BBC-880E-E66347D52EC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Contas" sheetId="1" r:id="rId1"/>
@@ -143,7 +143,7 @@
     <t>HP Pro</t>
   </si>
   <si>
-    <t>Printscreen5</t>
+    <t>Printscreen51</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Adicionado comando em java para esperar antes de tirar a screenshot do cenario de falha no pesquisar produto pela lupa.
</commit_message>
<xml_diff>
--- a/target/Excel/Dados.xlsx
+++ b/target/Excel/Dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus.vieira\ProjetoAdvantageBDD\AdvantageShopBDD\target\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F7CC65-620D-4817-BB7E-C492EF1E803C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6738F22F-1BED-49BF-9692-C4282C3FC558}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E0E69BFF-8C0C-4BBC-880E-E66347D52EC9}"/>
+    <workbookView xWindow="1995" yWindow="1560" windowWidth="16200" windowHeight="9360" xr2:uid="{E0E69BFF-8C0C-4BBC-880E-E66347D52EC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Contas" sheetId="1" r:id="rId1"/>
@@ -143,7 +143,7 @@
     <t>HP Pro</t>
   </si>
   <si>
-    <t>Printscreen51</t>
+    <t>Printscren003</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Alterado a feature de criar conta a parte do contexto pensando em futuras modificações, e alterado o metodo de report.
</commit_message>
<xml_diff>
--- a/target/Excel/Dados.xlsx
+++ b/target/Excel/Dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus.vieira\ProjetoAdvantageBDD\AdvantageShopBDD\target\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6738F22F-1BED-49BF-9692-C4282C3FC558}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D03DE0D-D2C3-482B-81B6-483F765BCAE8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1995" yWindow="1560" windowWidth="16200" windowHeight="9360" xr2:uid="{E0E69BFF-8C0C-4BBC-880E-E66347D52EC9}"/>
   </bookViews>
@@ -143,7 +143,7 @@
     <t>HP Pro</t>
   </si>
   <si>
-    <t>Printscren003</t>
+    <t>Printscr9991</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Renomeado os pacotes de Excel, ScreenSHot e stepDefinition, pois os mesmo estavam com os nomes errados.
</commit_message>
<xml_diff>
--- a/target/Excel/Dados.xlsx
+++ b/target/Excel/Dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus.vieira\ProjetoAdvantageBDD\AdvantageShopBDD\target\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D03DE0D-D2C3-482B-81B6-483F765BCAE8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADAE38EF-EDBD-444F-894E-0317111F2F2F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1995" yWindow="1560" windowWidth="16200" windowHeight="9360" xr2:uid="{E0E69BFF-8C0C-4BBC-880E-E66347D52EC9}"/>
   </bookViews>
@@ -143,7 +143,7 @@
     <t>HP Pro</t>
   </si>
   <si>
-    <t>Printscr9991</t>
+    <t>Printscr9992</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
acrescentado dependencia ao pom e alterado o step de pesquisar na pagina inicial do teste.
</commit_message>
<xml_diff>
--- a/target/Excel/Dados.xlsx
+++ b/target/Excel/Dados.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus.vieira\ProjetoAdvantageBDD\AdvantageShopBDD\target\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus.vieira\Desktop\projeto\AdvantageShopBDD\target\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADAE38EF-EDBD-444F-894E-0317111F2F2F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{299BB46C-5AF9-4F23-925E-65A9055A96B2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1995" yWindow="1560" windowWidth="16200" windowHeight="9360" xr2:uid="{E0E69BFF-8C0C-4BBC-880E-E66347D52EC9}"/>
   </bookViews>
@@ -143,7 +143,7 @@
     <t>HP Pro</t>
   </si>
   <si>
-    <t>Printscr9992</t>
+    <t>Mattthew</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Refatorado o codigo e aplicado boas praticas.
</commit_message>
<xml_diff>
--- a/target/Excel/Dados.xlsx
+++ b/target/Excel/Dados.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus.vieira\Desktop\projeto\AdvantageShopBDD\target\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus.vieira\Desktop\Projeto\AdvantageShopBDD\target\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{299BB46C-5AF9-4F23-925E-65A9055A96B2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A8FCD9-83C2-4197-9AD8-B5A70872158E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1995" yWindow="1560" windowWidth="16200" windowHeight="9360" xr2:uid="{E0E69BFF-8C0C-4BBC-880E-E66347D52EC9}"/>
+    <workbookView xWindow="1860" yWindow="2205" windowWidth="15375" windowHeight="7875" xr2:uid="{E0E69BFF-8C0C-4BBC-880E-E66347D52EC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Contas" sheetId="1" r:id="rId1"/>
@@ -143,7 +143,7 @@
     <t>HP Pro</t>
   </si>
   <si>
-    <t>Mattthew</t>
+    <t>Cachorro001</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Removido logs dos resultados anteriores dos testes.
</commit_message>
<xml_diff>
--- a/target/Excel/Dados.xlsx
+++ b/target/Excel/Dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus.vieira\Desktop\Projeto\AdvantageShopBDD\target\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A8FCD9-83C2-4197-9AD8-B5A70872158E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B6EBEB-1E3F-46FB-B84F-0ACA5FB0DA66}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="2205" windowWidth="15375" windowHeight="7875" xr2:uid="{E0E69BFF-8C0C-4BBC-880E-E66347D52EC9}"/>
   </bookViews>
@@ -143,7 +143,7 @@
     <t>HP Pro</t>
   </si>
   <si>
-    <t>Cachorro001</t>
+    <t>AmimVi2997</t>
   </si>
 </sst>
 </file>

</xml_diff>